<commit_message>
add excel export to linear model
</commit_message>
<xml_diff>
--- a/Instances.xlsx
+++ b/Instances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mon Drive\COURS\GI06\GP30\Projet\Pricing_GP30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDFB2FE-3B7C-4061-B6FD-33F3335459CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24ACC11-50FC-4C1B-BA6D-B024F069F723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="5025" windowWidth="29040" windowHeight="15840" xr2:uid="{48ACF279-63E4-478A-B5A4-CD8783F5C483}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{48ACF279-63E4-478A-B5A4-CD8783F5C483}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>CONSUMERS</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>ini</t>
+  </si>
+  <si>
+    <t>ini_2</t>
   </si>
 </sst>
 </file>
@@ -173,8 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD131D6-5F44-471A-BADA-8185BBB3E399}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -664,6 +668,41 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1">
+        <v>9</v>
+      </c>
+      <c r="K7" s="1">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add gusek model and save excel file for lingo
</commit_message>
<xml_diff>
--- a/Instances.xlsx
+++ b/Instances.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mon Drive\COURS\GI06\GP30\Projet\Pricing_GP30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24ACC11-50FC-4C1B-BA6D-B024F069F723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF607B2-05A7-42D8-8104-29F263255727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{48ACF279-63E4-478A-B5A4-CD8783F5C483}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -673,34 +673,34 @@
         <v>32</v>
       </c>
       <c r="B7" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
-        <v>6</v>
-      </c>
       <c r="E7" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H7" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1">
         <v>12</v>
-      </c>
-      <c r="J7" s="1">
-        <v>9</v>
-      </c>
-      <c r="K7" s="1">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>